<commit_message>
added first profiles for sarcoma staging
</commit_message>
<xml_diff>
--- a/src-models/IDEA4RC_DM_V1.xlsx
+++ b/src-models/IDEA4RC_DM_V1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <workbookPr codeName="Questa_cartella_di_lavoro"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\idea4rc\src-models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7F167A-FC0B-42E3-9DD0-3D90A9232D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22F4BA0-7C92-4C85-B7D7-AC29047EA26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{E806E8D1-DF08-4AF4-B4D7-368F8D75B1D5}"/>
+    <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" firstSheet="1" activeTab="12" xr2:uid="{E806E8D1-DF08-4AF4-B4D7-368F8D75B1D5}"/>
   </bookViews>
   <sheets>
     <sheet name="HOWTO" sheetId="1" r:id="rId1"/>
@@ -63,6 +63,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={75CF20DE-6B95-422A-8C45-A17581BF5825}</author>
+  </authors>
+  <commentList>
+    <comment ref="M4" authorId="0" shapeId="0" xr:uid="{75CF20DE-6B95-422A-8C45-A17581BF5825}">
+      <text>
+        <t>[Commento in thread]
+La versione di Excel in uso consente di leggere questo commento in thread, ma tutte le modifiche a esso apportate verranno rimosse se il file viene aperto in una versione più recente di Excel. Ulteriori informazioni: https://go.microsoft.com/fwlink/?linkid=870924
+Commento:
+Invasive is a disease extent</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4527" uniqueCount="1819">
   <si>
@@ -24306,7 +24324,7 @@
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="yyyy/m"/>
   </numFmts>
-  <fonts count="106">
+  <fonts count="107">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -25005,8 +25023,14 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -25106,6 +25130,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -25267,7 +25297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="261">
+  <cellXfs count="262">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -25904,6 +25934,12 @@
     <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -25963,10 +25999,7 @@
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -26330,6 +26363,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Giorgio Cangioli" id="{54F6A552-3817-476D-9C37-DE9621756D57}" userId="S::giorgio.cangioli@hl7europe.onmicrosoft.com::3df7a51e-573e-486b-8851-f60d1893331a" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -26526,9 +26565,17 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="M4" dT="2024-07-03T16:46:57.35" personId="{54F6A552-3817-476D-9C37-DE9621756D57}" id="{75CF20DE-6B95-422A-8C45-A17581BF5825}">
+    <text>Invasive is a disease extent</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B2:B6"/>
@@ -26565,7 +26612,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio10">
     <tabColor rgb="FFE69138"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -29011,7 +29058,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio11">
     <tabColor rgb="FFF7981D"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -29281,7 +29328,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio12">
     <tabColor rgb="FF45818E"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -30276,14 +30323,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr codeName="Foglio13">
     <tabColor rgb="FF45818E"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -30469,7 +30518,7 @@
         <v>1026</v>
       </c>
       <c r="L4" s="11"/>
-      <c r="M4" s="84" t="s">
+      <c r="M4" s="261" t="s">
         <v>1027</v>
       </c>
       <c r="N4" s="11"/>
@@ -30482,7 +30531,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="39">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="10" t="s">
         <v>1029</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -31038,12 +31087,13 @@
     <hyperlink ref="M14" r:id="rId13" xr:uid="{00000000-0004-0000-0C00-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId14"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio14">
     <tabColor rgb="FF45818E"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -31550,7 +31600,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio15">
     <tabColor rgb="FFA64D79"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -32328,7 +32378,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio16">
     <tabColor rgb="FF6AA84F"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -33730,7 +33780,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio17">
     <tabColor rgb="FF6AA84F"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -34396,7 +34446,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio18">
     <tabColor rgb="FF6AA84F"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -35771,7 +35821,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio19">
     <tabColor rgb="FF6AA84F"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -36139,7 +36189,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio2">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:H95"/>
@@ -38477,7 +38527,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio20">
     <tabColor rgb="FF6AA84F"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -38800,7 +38850,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio21">
     <tabColor rgb="FF6AA84F"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -38972,7 +39022,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio22">
     <tabColor rgb="FF6AA84F"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -39195,7 +39245,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio23">
     <tabColor rgb="FFA61C00"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -39464,7 +39514,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio24">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C1"/>
@@ -39491,7 +39541,7 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio25">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:B32"/>
@@ -39750,7 +39800,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio26">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:F104"/>
@@ -39915,13 +39965,13 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.25">
-      <c r="A11" s="237" t="s">
+      <c r="A11" s="239" t="s">
         <v>1398</v>
       </c>
-      <c r="B11" s="239" t="s">
+      <c r="B11" s="241" t="s">
         <v>1399</v>
       </c>
-      <c r="C11" s="240" t="s">
+      <c r="C11" s="242" t="s">
         <v>1400</v>
       </c>
       <c r="E11" s="161" t="s">
@@ -39932,9 +39982,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.25">
-      <c r="A12" s="235"/>
-      <c r="B12" s="235"/>
-      <c r="C12" s="235"/>
+      <c r="A12" s="237"/>
+      <c r="B12" s="237"/>
+      <c r="C12" s="237"/>
       <c r="E12" s="161" t="s">
         <v>1402</v>
       </c>
@@ -39943,9 +39993,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.25">
-      <c r="A13" s="235"/>
-      <c r="B13" s="235"/>
-      <c r="C13" s="235"/>
+      <c r="A13" s="237"/>
+      <c r="B13" s="237"/>
+      <c r="C13" s="237"/>
       <c r="E13" s="161" t="s">
         <v>1403</v>
       </c>
@@ -39954,9 +40004,9 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.25">
-      <c r="A14" s="238"/>
-      <c r="B14" s="235"/>
-      <c r="C14" s="235"/>
+      <c r="A14" s="240"/>
+      <c r="B14" s="237"/>
+      <c r="C14" s="237"/>
       <c r="E14" s="161" t="s">
         <v>1404</v>
       </c>
@@ -39965,13 +40015,13 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.25">
-      <c r="A15" s="241" t="s">
+      <c r="A15" s="243" t="s">
         <v>1405</v>
       </c>
-      <c r="B15" s="239" t="s">
+      <c r="B15" s="241" t="s">
         <v>1406</v>
       </c>
-      <c r="C15" s="236">
+      <c r="C15" s="238">
         <v>2246668</v>
       </c>
       <c r="E15" s="161" t="s">
@@ -39982,9 +40032,9 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="14.25">
-      <c r="A16" s="238"/>
-      <c r="B16" s="238"/>
-      <c r="C16" s="238"/>
+      <c r="A16" s="240"/>
+      <c r="B16" s="240"/>
+      <c r="C16" s="240"/>
       <c r="E16" s="161" t="s">
         <v>1409</v>
       </c>
@@ -40087,13 +40137,13 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.25">
-      <c r="A23" s="241" t="s">
+      <c r="A23" s="243" t="s">
         <v>1422</v>
       </c>
-      <c r="B23" s="239" t="s">
+      <c r="B23" s="241" t="s">
         <v>1423</v>
       </c>
-      <c r="C23" s="240" t="s">
+      <c r="C23" s="242" t="s">
         <v>1424</v>
       </c>
       <c r="E23" s="161" t="s">
@@ -40104,9 +40154,9 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.25">
-      <c r="A24" s="235"/>
-      <c r="B24" s="235"/>
-      <c r="C24" s="235"/>
+      <c r="A24" s="237"/>
+      <c r="B24" s="237"/>
+      <c r="C24" s="237"/>
       <c r="E24" s="161" t="s">
         <v>1426</v>
       </c>
@@ -40115,18 +40165,18 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.5">
-      <c r="A25" s="235"/>
-      <c r="B25" s="235"/>
-      <c r="C25" s="235"/>
+      <c r="A25" s="237"/>
+      <c r="B25" s="237"/>
+      <c r="C25" s="237"/>
       <c r="E25" s="158" t="s">
         <v>1427</v>
       </c>
       <c r="F25" s="159"/>
     </row>
     <row r="26" spans="1:6" ht="14.25">
-      <c r="A26" s="238"/>
-      <c r="B26" s="235"/>
-      <c r="C26" s="235"/>
+      <c r="A26" s="240"/>
+      <c r="B26" s="237"/>
+      <c r="C26" s="237"/>
       <c r="E26" s="161" t="s">
         <v>1428</v>
       </c>
@@ -40201,13 +40251,13 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="14.25">
-      <c r="A31" s="239" t="s">
+      <c r="A31" s="241" t="s">
         <v>1439</v>
       </c>
-      <c r="B31" s="239" t="s">
+      <c r="B31" s="241" t="s">
         <v>1440</v>
       </c>
-      <c r="C31" s="236">
+      <c r="C31" s="238">
         <v>2419793</v>
       </c>
       <c r="E31" s="161" t="s">
@@ -40218,9 +40268,9 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="14.25">
-      <c r="A32" s="238"/>
-      <c r="B32" s="238"/>
-      <c r="C32" s="238"/>
+      <c r="A32" s="240"/>
+      <c r="B32" s="240"/>
+      <c r="C32" s="240"/>
       <c r="E32" s="161" t="s">
         <v>1442</v>
       </c>
@@ -40361,13 +40411,13 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="14.25">
-      <c r="A41" s="234" t="s">
+      <c r="A41" s="236" t="s">
         <v>1462</v>
       </c>
-      <c r="B41" s="234" t="s">
+      <c r="B41" s="236" t="s">
         <v>1463</v>
       </c>
-      <c r="C41" s="236">
+      <c r="C41" s="238">
         <v>2571734</v>
       </c>
       <c r="E41" s="161" t="s">
@@ -40378,9 +40428,9 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="14.25">
-      <c r="A42" s="235"/>
-      <c r="B42" s="235"/>
-      <c r="C42" s="235"/>
+      <c r="A42" s="237"/>
+      <c r="B42" s="237"/>
+      <c r="C42" s="237"/>
       <c r="E42" s="161" t="s">
         <v>1465</v>
       </c>
@@ -41108,7 +41158,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio27">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:F79"/>
@@ -41146,22 +41196,22 @@
       <c r="F2" s="186"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A3" s="245" t="s">
+      <c r="A3" s="247" t="s">
         <v>1560</v>
       </c>
-      <c r="B3" s="246"/>
-      <c r="C3" s="246"/>
-      <c r="D3" s="246"/>
+      <c r="B3" s="248"/>
+      <c r="C3" s="248"/>
+      <c r="D3" s="248"/>
       <c r="E3" s="186"/>
       <c r="F3" s="187" t="s">
         <v>1561</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A4" s="246"/>
-      <c r="B4" s="246"/>
-      <c r="C4" s="246"/>
-      <c r="D4" s="246"/>
+      <c r="A4" s="248"/>
+      <c r="B4" s="248"/>
+      <c r="C4" s="248"/>
+      <c r="D4" s="248"/>
       <c r="E4" s="186"/>
       <c r="F4" s="188" t="s">
         <v>1562</v>
@@ -41195,7 +41245,7 @@
       <c r="C6" s="194" t="s">
         <v>1570</v>
       </c>
-      <c r="D6" s="247" t="s">
+      <c r="D6" s="249" t="s">
         <v>1571</v>
       </c>
       <c r="E6" s="186"/>
@@ -41211,7 +41261,7 @@
       <c r="C7" s="194" t="s">
         <v>1574</v>
       </c>
-      <c r="D7" s="248"/>
+      <c r="D7" s="250"/>
       <c r="E7" s="186"/>
       <c r="F7" s="196" t="s">
         <v>1575</v>
@@ -41225,7 +41275,7 @@
       <c r="C8" s="194" t="s">
         <v>1577</v>
       </c>
-      <c r="D8" s="248"/>
+      <c r="D8" s="250"/>
       <c r="E8" s="186"/>
       <c r="F8" s="196" t="s">
         <v>1578</v>
@@ -41239,7 +41289,7 @@
       <c r="C9" s="197" t="s">
         <v>1580</v>
       </c>
-      <c r="D9" s="248"/>
+      <c r="D9" s="250"/>
       <c r="E9" s="186"/>
       <c r="F9" s="196" t="s">
         <v>1581</v>
@@ -41253,7 +41303,7 @@
       <c r="C10" s="200" t="s">
         <v>1583</v>
       </c>
-      <c r="D10" s="248"/>
+      <c r="D10" s="250"/>
       <c r="E10" s="186"/>
       <c r="F10" s="196" t="s">
         <v>1584</v>
@@ -41269,7 +41319,7 @@
       <c r="C11" s="197" t="s">
         <v>1587</v>
       </c>
-      <c r="D11" s="248"/>
+      <c r="D11" s="250"/>
       <c r="E11" s="186"/>
       <c r="F11" s="191" t="s">
         <v>1588</v>
@@ -41283,7 +41333,7 @@
       <c r="C12" s="197" t="s">
         <v>1590</v>
       </c>
-      <c r="D12" s="248"/>
+      <c r="D12" s="250"/>
       <c r="E12" s="186"/>
       <c r="F12" s="196" t="s">
         <v>1591</v>
@@ -41297,7 +41347,7 @@
       <c r="C13" s="194" t="s">
         <v>1593</v>
       </c>
-      <c r="D13" s="248"/>
+      <c r="D13" s="250"/>
       <c r="E13" s="186"/>
       <c r="F13" s="196" t="s">
         <v>1594</v>
@@ -41311,7 +41361,7 @@
       <c r="C14" s="200" t="s">
         <v>1596</v>
       </c>
-      <c r="D14" s="248"/>
+      <c r="D14" s="250"/>
       <c r="E14" s="186"/>
       <c r="F14" s="196" t="s">
         <v>1597</v>
@@ -41325,7 +41375,7 @@
       <c r="C15" s="194" t="s">
         <v>1599</v>
       </c>
-      <c r="D15" s="248"/>
+      <c r="D15" s="250"/>
       <c r="E15" s="186"/>
       <c r="F15" s="196" t="s">
         <v>1600</v>
@@ -41339,7 +41389,7 @@
       <c r="C16" s="194" t="s">
         <v>1602</v>
       </c>
-      <c r="D16" s="248"/>
+      <c r="D16" s="250"/>
       <c r="E16" s="186"/>
       <c r="F16" s="196" t="s">
         <v>1603</v>
@@ -41353,7 +41403,7 @@
       <c r="C17" s="204" t="s">
         <v>1605</v>
       </c>
-      <c r="D17" s="248"/>
+      <c r="D17" s="250"/>
       <c r="E17" s="186"/>
       <c r="F17" s="191" t="s">
         <v>1606</v>
@@ -41367,7 +41417,7 @@
       <c r="C18" s="204" t="s">
         <v>1608</v>
       </c>
-      <c r="D18" s="249"/>
+      <c r="D18" s="251"/>
       <c r="E18" s="186"/>
       <c r="F18" s="196" t="s">
         <v>1609</v>
@@ -41384,12 +41434,12 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A20" s="245" t="s">
+      <c r="A20" s="247" t="s">
         <v>1611</v>
       </c>
-      <c r="B20" s="246"/>
-      <c r="C20" s="246"/>
-      <c r="D20" s="246"/>
+      <c r="B20" s="248"/>
+      <c r="C20" s="248"/>
+      <c r="D20" s="248"/>
       <c r="E20" s="186"/>
       <c r="F20" s="196" t="s">
         <v>1612</v>
@@ -41423,7 +41473,7 @@
       <c r="C22" s="207" t="s">
         <v>1618</v>
       </c>
-      <c r="D22" s="250" t="s">
+      <c r="D22" s="252" t="s">
         <v>1619</v>
       </c>
       <c r="E22" s="186"/>
@@ -41439,7 +41489,7 @@
       <c r="C23" s="208" t="s">
         <v>1621</v>
       </c>
-      <c r="D23" s="248"/>
+      <c r="D23" s="250"/>
       <c r="E23" s="186"/>
       <c r="F23" s="209" t="s">
         <v>1622</v>
@@ -41453,7 +41503,7 @@
       <c r="C24" s="207" t="s">
         <v>1624</v>
       </c>
-      <c r="D24" s="248"/>
+      <c r="D24" s="250"/>
       <c r="E24" s="186"/>
       <c r="F24" s="210" t="s">
         <v>1625</v>
@@ -41467,7 +41517,7 @@
       <c r="C25" s="211" t="s">
         <v>1599</v>
       </c>
-      <c r="D25" s="248"/>
+      <c r="D25" s="250"/>
       <c r="E25" s="186"/>
       <c r="F25" s="196" t="s">
         <v>1626</v>
@@ -41481,7 +41531,7 @@
       <c r="C26" s="211" t="s">
         <v>1602</v>
       </c>
-      <c r="D26" s="248"/>
+      <c r="D26" s="250"/>
       <c r="E26" s="186"/>
       <c r="F26" s="196" t="s">
         <v>1627</v>
@@ -41495,7 +41545,7 @@
       <c r="C27" s="211" t="s">
         <v>1605</v>
       </c>
-      <c r="D27" s="248"/>
+      <c r="D27" s="250"/>
       <c r="E27" s="186"/>
       <c r="F27" s="191" t="s">
         <v>1628</v>
@@ -41509,7 +41559,7 @@
       <c r="C28" s="211" t="s">
         <v>1608</v>
       </c>
-      <c r="D28" s="248"/>
+      <c r="D28" s="250"/>
       <c r="E28" s="186"/>
       <c r="F28" s="209" t="s">
         <v>1629</v>
@@ -41523,7 +41573,7 @@
       <c r="C29" s="212" t="s">
         <v>1631</v>
       </c>
-      <c r="D29" s="248"/>
+      <c r="D29" s="250"/>
       <c r="E29" s="186"/>
       <c r="F29" s="196" t="s">
         <v>1632</v>
@@ -41537,7 +41587,7 @@
       <c r="C30" s="207" t="s">
         <v>1634</v>
       </c>
-      <c r="D30" s="248"/>
+      <c r="D30" s="250"/>
       <c r="E30" s="186"/>
       <c r="F30" s="213" t="s">
         <v>1635</v>
@@ -41551,7 +41601,7 @@
       <c r="C31" s="212" t="s">
         <v>1637</v>
       </c>
-      <c r="D31" s="248"/>
+      <c r="D31" s="250"/>
       <c r="E31" s="186"/>
       <c r="F31" s="191" t="s">
         <v>1638</v>
@@ -41565,7 +41615,7 @@
       <c r="C32" s="214" t="s">
         <v>1640</v>
       </c>
-      <c r="D32" s="249"/>
+      <c r="D32" s="251"/>
       <c r="E32" s="186"/>
       <c r="F32" s="196" t="s">
         <v>1641</v>
@@ -41581,7 +41631,7 @@
       <c r="C33" s="207" t="s">
         <v>1618</v>
       </c>
-      <c r="D33" s="251" t="s">
+      <c r="D33" s="253" t="s">
         <v>1643</v>
       </c>
       <c r="E33" s="186"/>
@@ -41597,7 +41647,7 @@
       <c r="C34" s="207" t="s">
         <v>1621</v>
       </c>
-      <c r="D34" s="248"/>
+      <c r="D34" s="250"/>
       <c r="E34" s="186"/>
       <c r="F34" s="196" t="s">
         <v>1645</v>
@@ -41611,7 +41661,7 @@
       <c r="C35" s="214" t="s">
         <v>1637</v>
       </c>
-      <c r="D35" s="249"/>
+      <c r="D35" s="251"/>
       <c r="E35" s="186"/>
       <c r="F35" s="196" t="s">
         <v>1646</v>
@@ -41656,7 +41706,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A39" s="252" t="s">
+      <c r="A39" s="254" t="s">
         <v>1653</v>
       </c>
       <c r="B39" s="185" t="s">
@@ -41672,7 +41722,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A40" s="235"/>
+      <c r="A40" s="237"/>
       <c r="B40" s="185" t="s">
         <v>1657</v>
       </c>
@@ -41686,7 +41736,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A41" s="235"/>
+      <c r="A41" s="237"/>
       <c r="B41" s="185" t="s">
         <v>1659</v>
       </c>
@@ -41700,7 +41750,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A42" s="235"/>
+      <c r="A42" s="237"/>
       <c r="B42" s="185" t="s">
         <v>1662</v>
       </c>
@@ -41714,7 +41764,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A43" s="235"/>
+      <c r="A43" s="237"/>
       <c r="B43" s="185" t="s">
         <v>1665</v>
       </c>
@@ -41728,7 +41778,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A44" s="235"/>
+      <c r="A44" s="237"/>
       <c r="B44" s="185" t="s">
         <v>1667</v>
       </c>
@@ -41742,7 +41792,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A45" s="238"/>
+      <c r="A45" s="240"/>
       <c r="B45" s="220" t="s">
         <v>1670</v>
       </c>
@@ -41756,7 +41806,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A46" s="252" t="s">
+      <c r="A46" s="254" t="s">
         <v>1673</v>
       </c>
       <c r="B46" s="185" t="s">
@@ -41772,7 +41822,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A47" s="235"/>
+      <c r="A47" s="237"/>
       <c r="B47" s="185" t="s">
         <v>1677</v>
       </c>
@@ -41786,7 +41836,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A48" s="235"/>
+      <c r="A48" s="237"/>
       <c r="B48" s="185" t="s">
         <v>1680</v>
       </c>
@@ -41800,7 +41850,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A49" s="235"/>
+      <c r="A49" s="237"/>
       <c r="B49" s="185" t="s">
         <v>1683</v>
       </c>
@@ -41814,7 +41864,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A50" s="235"/>
+      <c r="A50" s="237"/>
       <c r="B50" s="185" t="s">
         <v>1686</v>
       </c>
@@ -41828,7 +41878,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A51" s="235"/>
+      <c r="A51" s="237"/>
       <c r="B51" s="185" t="s">
         <v>1689</v>
       </c>
@@ -41842,7 +41892,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A52" s="235"/>
+      <c r="A52" s="237"/>
       <c r="B52" s="185" t="s">
         <v>1692</v>
       </c>
@@ -41856,7 +41906,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="14.75">
-      <c r="A53" s="235"/>
+      <c r="A53" s="237"/>
       <c r="B53" s="185" t="s">
         <v>1695</v>
       </c>
@@ -41870,7 +41920,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="14.75">
-      <c r="A54" s="235"/>
+      <c r="A54" s="237"/>
       <c r="B54" s="185" t="s">
         <v>1698</v>
       </c>
@@ -41884,7 +41934,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="14.75">
-      <c r="A55" s="235"/>
+      <c r="A55" s="237"/>
       <c r="B55" s="185" t="s">
         <v>1701</v>
       </c>
@@ -41898,7 +41948,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="14.75">
-      <c r="A56" s="235"/>
+      <c r="A56" s="237"/>
       <c r="B56" s="185" t="s">
         <v>1704</v>
       </c>
@@ -41912,7 +41962,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="14.75">
-      <c r="A57" s="235"/>
+      <c r="A57" s="237"/>
       <c r="B57" s="185" t="s">
         <v>1707</v>
       </c>
@@ -41926,7 +41976,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="14.75">
-      <c r="A58" s="235"/>
+      <c r="A58" s="237"/>
       <c r="B58" s="185" t="s">
         <v>1710</v>
       </c>
@@ -41940,7 +41990,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="14.75">
-      <c r="A59" s="235"/>
+      <c r="A59" s="237"/>
       <c r="B59" s="185" t="s">
         <v>1713</v>
       </c>
@@ -41954,7 +42004,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="14.75">
-      <c r="A60" s="238"/>
+      <c r="A60" s="240"/>
       <c r="B60" s="220" t="s">
         <v>1716</v>
       </c>
@@ -41968,7 +42018,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="14.75">
-      <c r="A61" s="242" t="s">
+      <c r="A61" s="244" t="s">
         <v>1718</v>
       </c>
       <c r="B61" s="185" t="s">
@@ -41984,7 +42034,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="14.75">
-      <c r="A62" s="243"/>
+      <c r="A62" s="245"/>
       <c r="B62" s="185" t="s">
         <v>1721</v>
       </c>
@@ -41998,7 +42048,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="14.75">
-      <c r="A63" s="243"/>
+      <c r="A63" s="245"/>
       <c r="B63" s="185" t="s">
         <v>1724</v>
       </c>
@@ -42010,7 +42060,7 @@
       <c r="F63" s="186"/>
     </row>
     <row r="64" spans="1:6" ht="14.75">
-      <c r="A64" s="243"/>
+      <c r="A64" s="245"/>
       <c r="B64" s="185" t="s">
         <v>1726</v>
       </c>
@@ -42022,7 +42072,7 @@
       <c r="F64" s="205"/>
     </row>
     <row r="65" spans="1:3" ht="14.75">
-      <c r="A65" s="243"/>
+      <c r="A65" s="245"/>
       <c r="B65" s="185" t="s">
         <v>1728</v>
       </c>
@@ -42031,7 +42081,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.75">
-      <c r="A66" s="243"/>
+      <c r="A66" s="245"/>
       <c r="B66" s="185" t="s">
         <v>1730</v>
       </c>
@@ -42040,7 +42090,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.75">
-      <c r="A67" s="243"/>
+      <c r="A67" s="245"/>
       <c r="B67" s="185" t="s">
         <v>1732</v>
       </c>
@@ -42049,7 +42099,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.75">
-      <c r="A68" s="243"/>
+      <c r="A68" s="245"/>
       <c r="B68" s="185" t="s">
         <v>1734</v>
       </c>
@@ -42058,7 +42108,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.75">
-      <c r="A69" s="243"/>
+      <c r="A69" s="245"/>
       <c r="B69" s="185" t="s">
         <v>1736</v>
       </c>
@@ -42067,7 +42117,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.75">
-      <c r="A70" s="243"/>
+      <c r="A70" s="245"/>
       <c r="B70" s="185" t="s">
         <v>1738</v>
       </c>
@@ -42076,7 +42126,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.75">
-      <c r="A71" s="244"/>
+      <c r="A71" s="246"/>
       <c r="B71" s="220" t="s">
         <v>1740</v>
       </c>
@@ -42085,7 +42135,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.75">
-      <c r="A72" s="242" t="s">
+      <c r="A72" s="244" t="s">
         <v>1742</v>
       </c>
       <c r="B72" s="185" t="s">
@@ -42096,7 +42146,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.75">
-      <c r="A73" s="243"/>
+      <c r="A73" s="245"/>
       <c r="B73" s="185" t="s">
         <v>1745</v>
       </c>
@@ -42105,7 +42155,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.75">
-      <c r="A74" s="243"/>
+      <c r="A74" s="245"/>
       <c r="B74" s="185" t="s">
         <v>1747</v>
       </c>
@@ -42114,7 +42164,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.75">
-      <c r="A75" s="244"/>
+      <c r="A75" s="246"/>
       <c r="B75" s="220" t="s">
         <v>1749</v>
       </c>
@@ -42123,7 +42173,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.75">
-      <c r="A76" s="242" t="s">
+      <c r="A76" s="244" t="s">
         <v>1751</v>
       </c>
       <c r="B76" s="185" t="s">
@@ -42134,7 +42184,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.75">
-      <c r="A77" s="243"/>
+      <c r="A77" s="245"/>
       <c r="B77" s="185" t="s">
         <v>1754</v>
       </c>
@@ -42143,7 +42193,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.75">
-      <c r="A78" s="243"/>
+      <c r="A78" s="245"/>
       <c r="B78" s="185" t="s">
         <v>1756</v>
       </c>
@@ -42152,7 +42202,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.75">
-      <c r="A79" s="244"/>
+      <c r="A79" s="246"/>
       <c r="B79" s="220" t="s">
         <v>1758</v>
       </c>
@@ -42179,7 +42229,7 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio28">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A2:G49"/>
@@ -42193,14 +42243,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="15.75" customHeight="1">
-      <c r="B2" s="253" t="s">
+      <c r="B2" s="255" t="s">
         <v>1760</v>
       </c>
-      <c r="C2" s="246"/>
-      <c r="D2" s="246"/>
-      <c r="E2" s="246"/>
-      <c r="F2" s="246"/>
-      <c r="G2" s="246"/>
+      <c r="C2" s="248"/>
+      <c r="D2" s="248"/>
+      <c r="E2" s="248"/>
+      <c r="F2" s="248"/>
+      <c r="G2" s="248"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" customHeight="1">
       <c r="B3" s="224"/>
@@ -42602,10 +42652,10 @@
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1">
       <c r="A33" s="222"/>
-      <c r="B33" s="254" t="s">
+      <c r="B33" s="256" t="s">
         <v>1791</v>
       </c>
-      <c r="C33" s="246"/>
+      <c r="C33" s="248"/>
       <c r="D33" s="223"/>
       <c r="E33" s="223"/>
     </row>
@@ -42856,7 +42906,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio29">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B2:C33"/>
@@ -42871,17 +42921,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B2" s="255" t="s">
+      <c r="B2" s="257" t="s">
         <v>1186</v>
       </c>
-      <c r="C2" s="246"/>
+      <c r="C2" s="248"/>
     </row>
     <row r="3" spans="2:3" ht="15.75" customHeight="1">
       <c r="B3" s="228"/>
       <c r="C3" s="227"/>
     </row>
     <row r="4" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B4" s="256" t="s">
+      <c r="B4" s="258" t="s">
         <v>1799</v>
       </c>
       <c r="C4" s="229" t="s">
@@ -42889,13 +42939,13 @@
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B5" s="238"/>
+      <c r="B5" s="240"/>
       <c r="C5" s="230" t="s">
         <v>1801</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B6" s="257" t="s">
+      <c r="B6" s="259" t="s">
         <v>1802</v>
       </c>
       <c r="C6" s="231" t="s">
@@ -42903,7 +42953,7 @@
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B7" s="238"/>
+      <c r="B7" s="240"/>
       <c r="C7" s="230" t="s">
         <v>1804</v>
       </c>
@@ -42965,8 +43015,8 @@
       </c>
     </row>
     <row r="33" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B33" s="258"/>
-      <c r="C33" s="246"/>
+      <c r="B33" s="260"/>
+      <c r="C33" s="248"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -42981,7 +43031,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio3">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G6"/>
@@ -43107,12 +43157,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr codeName="Foglio4" filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
@@ -43478,7 +43528,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="39">
-      <c r="A19" s="259" t="s">
+      <c r="A19" s="234" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="36" t="s">
@@ -44730,7 +44780,7 @@
       </c>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="260" t="s">
+      <c r="A82" s="235" t="s">
         <v>11</v>
       </c>
       <c r="B82" s="10" t="s">
@@ -44770,7 +44820,7 @@
       </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="260" t="s">
+      <c r="A84" s="235" t="s">
         <v>11</v>
       </c>
       <c r="B84" s="10" t="s">
@@ -45667,7 +45717,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio5">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1"/>
@@ -45686,7 +45736,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio6">
     <tabColor rgb="FF674EA7"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -48109,7 +48159,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio7">
     <tabColor rgb="FF674EA7"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -48528,7 +48578,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio8">
     <tabColor rgb="FF674EA7"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -48659,7 +48709,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Foglio9">
     <tabColor rgb="FF674EA7"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>